<commit_message>
Correção Pom para pipe
</commit_message>
<xml_diff>
--- a/src/test/resources/armazenador/IncluirCNPJs_Ofertas.xlsx
+++ b/src/test/resources/armazenador/IncluirCNPJs_Ofertas.xlsx
@@ -874,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK23"/>
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1099,7 +1099,7 @@
     <row r="16" spans="1:27">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1169,19 +1169,165 @@
     <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="C3:C26">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C37">
       <formula1>Plans</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H3:H26">
+    <dataValidation type="list" allowBlank="1" sqref="H3:H37">
       <formula1>Channels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F3:F26">
+    <dataValidation type="list" allowBlank="1" sqref="F3:F37">
       <formula1>Sheet2list</formula1>
     </dataValidation>
   </dataValidations>
@@ -1198,7 +1344,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G3:G22</xm:sqref>
+          <xm:sqref>G3:G37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Testes de Delivery Sprint 57
</commit_message>
<xml_diff>
--- a/src/test/resources/armazenador/IncluirCNPJs_Ofertas.xlsx
+++ b/src/test/resources/armazenador/IncluirCNPJs_Ofertas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="3990" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planos" sheetId="1" r:id="rId1"/>
@@ -874,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK37"/>
+  <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:H37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -964,7 +964,7 @@
         <v>44013</v>
       </c>
       <c r="E3" s="10">
-        <v>44053</v>
+        <v>44418</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>12</v>
@@ -1099,7 +1099,7 @@
     <row r="16" spans="1:27">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1169,165 +1169,19 @@
     <row r="23" spans="1:8">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="10"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="10"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="10"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="10"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="10"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="C3:C37">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C26">
       <formula1>Plans</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H3:H37">
+    <dataValidation type="list" allowBlank="1" sqref="H3:H26">
       <formula1>Channels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F3:F37">
+    <dataValidation type="list" allowBlank="1" sqref="F3:F26">
       <formula1>Sheet2list</formula1>
     </dataValidation>
   </dataValidations>
@@ -1344,7 +1198,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G3:G37</xm:sqref>
+          <xm:sqref>G3:G22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>